<commit_message>
scenarios 1 to 4 for glm and
</commit_message>
<xml_diff>
--- a/output/reports/Report_20jun25.xlsx
+++ b/output/reports/Report_20jun25.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\HCHS\STATISTICS\GRAS\QAngarita\HCHS_simulation\output\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1666A6-5664-469A-9FF7-B405610D99F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05EB477D-D4BE-4B69-B5F9-3BBF77607F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6855" yWindow="90" windowWidth="21600" windowHeight="12795" xr2:uid="{1D0456FE-5D68-4C25-AB8B-B6F8C81606F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1D0456FE-5D68-4C25-AB8B-B6F8C81606F9}"/>
   </bookViews>
   <sheets>
     <sheet name="RR_glm" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="29">
   <si>
     <t>Intercept</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>[4][PROC REGRESS][IND CORR][NO MI]bghhsub_s2_nr_nradj][SUDAAN TRUE]</t>
+  </si>
+  <si>
+    <t>[3][PROC REGRESS][IND CORR][MI V2][wn_3][SUDAAN TRUE]</t>
+  </si>
+  <si>
+    <t>[3][PROC REGRESS][EXCH CORR][MI V2][wn_3][SUDAAN TRUE]</t>
   </si>
 </sst>
 </file>
@@ -222,7 +228,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="89">
+  <dxfs count="80">
     <dxf>
       <fill>
         <patternFill>
@@ -465,69 +471,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1161,10 +1104,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1548F76D-12E1-450F-93BE-034FF2CA0476}">
-  <dimension ref="A1:AV34"/>
+  <dimension ref="A1:AV44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2305,7 +2248,7 @@
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="C24" s="13" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
@@ -2317,7 +2260,7 @@
       <c r="K24" s="13"/>
       <c r="L24" s="13"/>
       <c r="N24" s="13" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="O24" s="13"/>
       <c r="P24" s="13"/>
@@ -2399,28 +2342,28 @@
         <v>107.08</v>
       </c>
       <c r="E26" s="9">
-        <v>102.75</v>
+        <v>106.129346</v>
       </c>
       <c r="F26" s="5">
-        <v>-4.32606</v>
+        <v>-0.94806000000000001</v>
       </c>
       <c r="G26" s="5">
-        <v>-4.0399999999999998E-2</v>
+        <v>-8.8500000000000002E-3</v>
       </c>
       <c r="H26" s="5">
-        <v>2.44</v>
+        <v>3.1468069999999999</v>
       </c>
       <c r="I26" s="5">
-        <v>2.19</v>
+        <v>3.0544099999999998</v>
       </c>
       <c r="J26" s="5">
-        <v>-0.10184</v>
+        <v>-2.9360000000000001E-2</v>
       </c>
       <c r="K26" s="7">
-        <v>0.48</v>
+        <v>0.96</v>
       </c>
       <c r="L26" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N26" s="1" t="s">
         <v>0</v>
@@ -2429,28 +2372,28 @@
         <v>106.81</v>
       </c>
       <c r="P26" s="9">
-        <v>99.62</v>
+        <v>106.276956</v>
       </c>
       <c r="Q26" s="10">
-        <v>-7.1952699999999998</v>
+        <v>-0.53549999999999998</v>
       </c>
       <c r="R26" s="10">
-        <v>-6.7360000000000003E-2</v>
+        <v>-5.0099999999999997E-3</v>
       </c>
       <c r="S26" s="10">
-        <v>3.88</v>
+        <v>4.2590110000000001</v>
       </c>
       <c r="T26" s="10">
-        <v>3.4</v>
+        <v>4.1199750000000002</v>
       </c>
       <c r="U26" s="10">
-        <v>-0.12357</v>
+        <v>-3.2649999999999998E-2</v>
       </c>
       <c r="V26" s="7">
-        <v>0.48</v>
+        <v>0.95</v>
       </c>
       <c r="W26" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
@@ -2461,28 +2404,28 @@
         <v>-4.7699999999999996</v>
       </c>
       <c r="E27" s="9">
-        <v>-4.76</v>
+        <v>-5.4797450000000003</v>
       </c>
       <c r="F27" s="5">
-        <v>5.9699999999999996E-3</v>
+        <v>-0.71109999999999995</v>
       </c>
       <c r="G27" s="5">
-        <v>-1.25E-3</v>
+        <v>0.14912</v>
       </c>
       <c r="H27" s="5">
-        <v>0.94</v>
+        <v>1.390611</v>
       </c>
       <c r="I27" s="5">
-        <v>0.89</v>
+        <v>1.3339099999999999</v>
       </c>
       <c r="J27" s="5">
-        <v>-5.28E-2</v>
+        <v>-4.0770000000000001E-2</v>
       </c>
       <c r="K27" s="7">
         <v>0.94</v>
       </c>
       <c r="L27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N27" s="1" t="s">
         <v>11</v>
@@ -2491,28 +2434,28 @@
         <v>-4.8</v>
       </c>
       <c r="P27" s="9">
-        <v>-5.0599999999999996</v>
+        <v>-5.3410200000000003</v>
       </c>
       <c r="Q27" s="10">
-        <v>-0.26543</v>
+        <v>-0.54174</v>
       </c>
       <c r="R27" s="10">
-        <v>5.5309999999999998E-2</v>
+        <v>0.11287999999999999</v>
       </c>
       <c r="S27" s="10">
-        <v>1.42</v>
+        <v>1.7073579999999999</v>
       </c>
       <c r="T27" s="10">
-        <v>1.31</v>
+        <v>1.6533599999999999</v>
       </c>
       <c r="U27" s="10">
-        <v>-7.7679999999999999E-2</v>
+        <v>-3.1629999999999998E-2</v>
       </c>
       <c r="V27" s="7">
-        <v>0.92</v>
+        <v>0.96</v>
       </c>
       <c r="W27" s="7">
-        <v>0.94</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
@@ -2523,28 +2466,28 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="E28" s="9">
-        <v>10.61</v>
+        <v>8.7944180000000003</v>
       </c>
       <c r="F28" s="5">
-        <v>1.9110100000000001</v>
+        <v>9.7720000000000001E-2</v>
       </c>
       <c r="G28" s="5">
-        <v>0.21973999999999999</v>
+        <v>1.124E-2</v>
       </c>
       <c r="H28" s="5">
-        <v>0.54</v>
+        <v>0.61224199999999995</v>
       </c>
       <c r="I28" s="5">
-        <v>0.52</v>
+        <v>0.63399000000000005</v>
       </c>
       <c r="J28" s="5">
-        <v>-3.7620000000000001E-2</v>
+        <v>3.5520000000000003E-2</v>
       </c>
       <c r="K28" s="7">
-        <v>0.03</v>
+        <v>0.95</v>
       </c>
       <c r="L28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N28" s="1" t="s">
         <v>12</v>
@@ -2553,28 +2496,28 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="P28" s="9">
-        <v>12.85</v>
+        <v>8.8040400000000005</v>
       </c>
       <c r="Q28" s="10">
-        <v>4.1439599999999999</v>
+        <v>0.10183</v>
       </c>
       <c r="R28" s="10">
-        <v>0.47620000000000001</v>
+        <v>1.17E-2</v>
       </c>
       <c r="S28" s="10">
-        <v>0.74</v>
+        <v>0.76390199999999997</v>
       </c>
       <c r="T28" s="10">
-        <v>0.71</v>
+        <v>0.75951000000000002</v>
       </c>
       <c r="U28" s="10">
-        <v>-4.6010000000000002E-2</v>
+        <v>-5.7499999999999999E-3</v>
       </c>
       <c r="V28" s="7">
-        <v>0</v>
+        <v>0.93</v>
       </c>
       <c r="W28" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
@@ -2585,28 +2528,28 @@
         <v>-1.61</v>
       </c>
       <c r="E29" s="9">
-        <v>-1.02</v>
+        <v>-1.2076309999999999</v>
       </c>
       <c r="F29" s="5">
-        <v>0.58933000000000002</v>
+        <v>0.40266000000000002</v>
       </c>
       <c r="G29" s="5">
-        <v>-0.36598000000000003</v>
+        <v>-0.25006</v>
       </c>
       <c r="H29" s="5">
-        <v>0.6</v>
+        <v>0.82627499999999998</v>
       </c>
       <c r="I29" s="5">
-        <v>0.55000000000000004</v>
+        <v>0.74576399999999998</v>
       </c>
       <c r="J29" s="5">
-        <v>-8.3599999999999994E-2</v>
+        <v>-9.7439999999999999E-2</v>
       </c>
       <c r="K29" s="7">
-        <v>0.8</v>
+        <v>0.92</v>
       </c>
       <c r="L29" s="2">
-        <v>0.42</v>
+        <v>0</v>
       </c>
       <c r="N29" s="1" t="s">
         <v>13</v>
@@ -2615,28 +2558,28 @@
         <v>-1.58</v>
       </c>
       <c r="P29" s="9">
-        <v>-0.54</v>
+        <v>-1.289026</v>
       </c>
       <c r="Q29" s="10">
-        <v>1.03694</v>
+        <v>0.29160000000000003</v>
       </c>
       <c r="R29" s="10">
-        <v>-0.65603</v>
+        <v>-0.18448000000000001</v>
       </c>
       <c r="S29" s="10">
-        <v>0.98</v>
+        <v>1.1253329999999999</v>
       </c>
       <c r="T29" s="10">
-        <v>0.88</v>
+        <v>1.020947</v>
       </c>
       <c r="U29" s="10">
-        <v>-0.10183</v>
+        <v>-9.2759999999999995E-2</v>
       </c>
       <c r="V29" s="7">
-        <v>0.75</v>
+        <v>0.94</v>
       </c>
       <c r="W29" s="7">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
@@ -2647,28 +2590,28 @@
         <v>-7.92</v>
       </c>
       <c r="E30" s="9">
-        <v>-9.82</v>
+        <v>-7.7106219999999999</v>
       </c>
       <c r="F30" s="5">
-        <v>-1.9097200000000001</v>
+        <v>0.20455000000000001</v>
       </c>
       <c r="G30" s="5">
-        <v>0.24127000000000001</v>
+        <v>-2.5839999999999998E-2</v>
       </c>
       <c r="H30" s="5">
-        <v>0.77</v>
+        <v>0.88131999999999999</v>
       </c>
       <c r="I30" s="5">
-        <v>0.69</v>
+        <v>0.83728400000000003</v>
       </c>
       <c r="J30" s="5">
-        <v>-9.894E-2</v>
+        <v>-4.9970000000000001E-2</v>
       </c>
       <c r="K30" s="7">
-        <v>0.24</v>
+        <v>0.9</v>
       </c>
       <c r="L30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N30" s="1" t="s">
         <v>14</v>
@@ -2677,28 +2620,28 @@
         <v>-7.78</v>
       </c>
       <c r="P30" s="9">
-        <v>-11.73</v>
+        <v>-7.6972670000000001</v>
       </c>
       <c r="Q30" s="10">
-        <v>-3.9555899999999999</v>
+        <v>7.9159999999999994E-2</v>
       </c>
       <c r="R30" s="10">
-        <v>0.50866</v>
+        <v>-1.018E-2</v>
       </c>
       <c r="S30" s="10">
-        <v>0.98</v>
+        <v>1.0350330000000001</v>
       </c>
       <c r="T30" s="10">
+        <v>1.002953</v>
+      </c>
+      <c r="U30" s="10">
+        <v>-3.099E-2</v>
+      </c>
+      <c r="V30" s="7">
         <v>0.93</v>
       </c>
-      <c r="U30" s="10">
-        <v>-4.5859999999999998E-2</v>
-      </c>
-      <c r="V30" s="7">
-        <v>0.04</v>
-      </c>
       <c r="W30" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
@@ -2709,28 +2652,28 @@
         <v>5.87</v>
       </c>
       <c r="E31" s="9">
-        <v>6.02</v>
+        <v>5.8917700000000002</v>
       </c>
       <c r="F31" s="5">
-        <v>0.14910000000000001</v>
+        <v>2.3630000000000002E-2</v>
       </c>
       <c r="G31" s="5">
-        <v>2.5409999999999999E-2</v>
+        <v>4.0299999999999997E-3</v>
       </c>
       <c r="H31" s="5">
-        <v>0.04</v>
+        <v>5.0598999999999998E-2</v>
       </c>
       <c r="I31" s="5">
-        <v>0.04</v>
+        <v>6.608E-2</v>
       </c>
       <c r="J31" s="5">
-        <v>4.419E-2</v>
+        <v>0.30596000000000001</v>
       </c>
       <c r="K31" s="7">
-        <v>0.05</v>
+        <v>0.98</v>
       </c>
       <c r="L31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N31" s="1" t="s">
         <v>15</v>
@@ -2739,28 +2682,28 @@
         <v>5.86</v>
       </c>
       <c r="P31" s="9">
-        <v>5.99</v>
+        <v>5.871804</v>
       </c>
       <c r="Q31" s="10">
-        <v>0.12862999999999999</v>
+        <v>7.3899999999999999E-3</v>
       </c>
       <c r="R31" s="10">
-        <v>2.1930000000000002E-2</v>
+        <v>1.2600000000000001E-3</v>
       </c>
       <c r="S31" s="10">
-        <v>0.03</v>
+        <v>5.8562000000000003E-2</v>
       </c>
       <c r="T31" s="10">
-        <v>0.04</v>
+        <v>7.6060000000000003E-2</v>
       </c>
       <c r="U31" s="10">
-        <v>0.10811</v>
+        <v>0.29881000000000002</v>
       </c>
       <c r="V31" s="7">
-        <v>0.02</v>
+        <v>0.98</v>
       </c>
       <c r="W31" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
@@ -2771,28 +2714,28 @@
         <v>0.03</v>
       </c>
       <c r="E32" s="9">
-        <v>0.02</v>
+        <v>1.3802E-2</v>
       </c>
       <c r="F32" s="5">
-        <v>-4.0499999999999998E-3</v>
+        <v>-1.461E-2</v>
       </c>
       <c r="G32" s="5">
-        <v>-0.14241999999999999</v>
+        <v>-0.51427999999999996</v>
       </c>
       <c r="H32" s="5">
-        <v>0.03</v>
+        <v>4.5643999999999997E-2</v>
       </c>
       <c r="I32" s="5">
-        <v>0.03</v>
+        <v>5.6280999999999998E-2</v>
       </c>
       <c r="J32" s="5">
-        <v>-4.9259999999999998E-2</v>
+        <v>0.23305000000000001</v>
       </c>
       <c r="K32" s="7">
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
       <c r="L32" s="2">
-        <v>0.14000000000000001</v>
+        <v>0</v>
       </c>
       <c r="N32" s="1" t="s">
         <v>16</v>
@@ -2801,178 +2744,740 @@
         <v>0.03</v>
       </c>
       <c r="P32" s="9">
+        <v>3.4111000000000002E-2</v>
+      </c>
+      <c r="Q32" s="10">
+        <v>2E-3</v>
+      </c>
+      <c r="R32" s="10">
+        <v>6.2370000000000002E-2</v>
+      </c>
+      <c r="S32" s="10">
+        <v>5.4664999999999998E-2</v>
+      </c>
+      <c r="T32" s="10">
+        <v>6.7529000000000006E-2</v>
+      </c>
+      <c r="U32" s="10">
+        <v>0.23533999999999999</v>
+      </c>
+      <c r="V32" s="7">
+        <v>0.98</v>
+      </c>
+      <c r="W32" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C34" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="N34" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="O34" s="13"/>
+      <c r="P34" s="13"/>
+      <c r="Q34" s="13"/>
+      <c r="R34" s="13"/>
+      <c r="S34" s="13"/>
+      <c r="T34" s="13"/>
+      <c r="U34" s="13"/>
+      <c r="V34" s="13"/>
+      <c r="W34" s="13"/>
+    </row>
+    <row r="35" spans="3:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="C35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L35" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O35" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P35" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="R35" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="T35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="U35" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="V35" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W35" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C36" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" s="7">
+        <v>107.08</v>
+      </c>
+      <c r="E36" s="9">
+        <v>102.75</v>
+      </c>
+      <c r="F36" s="5">
+        <v>-4.32606</v>
+      </c>
+      <c r="G36" s="5">
+        <v>-4.0399999999999998E-2</v>
+      </c>
+      <c r="H36" s="5">
+        <v>2.44</v>
+      </c>
+      <c r="I36" s="5">
+        <v>2.19</v>
+      </c>
+      <c r="J36" s="5">
+        <v>-0.10184</v>
+      </c>
+      <c r="K36" s="7">
+        <v>0.48</v>
+      </c>
+      <c r="L36" s="2">
+        <v>1</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O36" s="7">
+        <v>106.81</v>
+      </c>
+      <c r="P36" s="9">
+        <v>99.62</v>
+      </c>
+      <c r="Q36" s="10">
+        <v>-7.1952699999999998</v>
+      </c>
+      <c r="R36" s="10">
+        <v>-6.7360000000000003E-2</v>
+      </c>
+      <c r="S36" s="10">
+        <v>3.88</v>
+      </c>
+      <c r="T36" s="10">
+        <v>3.4</v>
+      </c>
+      <c r="U36" s="10">
+        <v>-0.12357</v>
+      </c>
+      <c r="V36" s="7">
+        <v>0.48</v>
+      </c>
+      <c r="W36" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C37" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="7">
+        <v>-4.7699999999999996</v>
+      </c>
+      <c r="E37" s="9">
+        <v>-4.76</v>
+      </c>
+      <c r="F37" s="5">
+        <v>5.9699999999999996E-3</v>
+      </c>
+      <c r="G37" s="5">
+        <v>-1.25E-3</v>
+      </c>
+      <c r="H37" s="5">
+        <v>0.94</v>
+      </c>
+      <c r="I37" s="5">
+        <v>0.89</v>
+      </c>
+      <c r="J37" s="5">
+        <v>-5.28E-2</v>
+      </c>
+      <c r="K37" s="7">
+        <v>0.94</v>
+      </c>
+      <c r="L37" s="2">
+        <v>1</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O37" s="7">
+        <v>-4.8</v>
+      </c>
+      <c r="P37" s="9">
+        <v>-5.0599999999999996</v>
+      </c>
+      <c r="Q37" s="10">
+        <v>-0.26543</v>
+      </c>
+      <c r="R37" s="10">
+        <v>5.5309999999999998E-2</v>
+      </c>
+      <c r="S37" s="10">
+        <v>1.42</v>
+      </c>
+      <c r="T37" s="10">
+        <v>1.31</v>
+      </c>
+      <c r="U37" s="10">
+        <v>-7.7679999999999999E-2</v>
+      </c>
+      <c r="V37" s="7">
+        <v>0.92</v>
+      </c>
+      <c r="W37" s="7">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="38" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C38" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="7">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="E38" s="9">
+        <v>10.61</v>
+      </c>
+      <c r="F38" s="5">
+        <v>1.9110100000000001</v>
+      </c>
+      <c r="G38" s="5">
+        <v>0.21973999999999999</v>
+      </c>
+      <c r="H38" s="5">
+        <v>0.54</v>
+      </c>
+      <c r="I38" s="5">
+        <v>0.52</v>
+      </c>
+      <c r="J38" s="5">
+        <v>-3.7620000000000001E-2</v>
+      </c>
+      <c r="K38" s="7">
+        <v>0.03</v>
+      </c>
+      <c r="L38" s="2">
+        <v>1</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O38" s="7">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="P38" s="9">
+        <v>12.85</v>
+      </c>
+      <c r="Q38" s="10">
+        <v>4.1439599999999999</v>
+      </c>
+      <c r="R38" s="10">
+        <v>0.47620000000000001</v>
+      </c>
+      <c r="S38" s="10">
+        <v>0.74</v>
+      </c>
+      <c r="T38" s="10">
+        <v>0.71</v>
+      </c>
+      <c r="U38" s="10">
+        <v>-4.6010000000000002E-2</v>
+      </c>
+      <c r="V38" s="7">
+        <v>0</v>
+      </c>
+      <c r="W38" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C39" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="7">
+        <v>-1.61</v>
+      </c>
+      <c r="E39" s="9">
+        <v>-1.02</v>
+      </c>
+      <c r="F39" s="5">
+        <v>0.58933000000000002</v>
+      </c>
+      <c r="G39" s="5">
+        <v>-0.36598000000000003</v>
+      </c>
+      <c r="H39" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="I39" s="5">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J39" s="5">
+        <v>-8.3599999999999994E-2</v>
+      </c>
+      <c r="K39" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="L39" s="2">
+        <v>0.42</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O39" s="7">
+        <v>-1.58</v>
+      </c>
+      <c r="P39" s="9">
+        <v>-0.54</v>
+      </c>
+      <c r="Q39" s="10">
+        <v>1.03694</v>
+      </c>
+      <c r="R39" s="10">
+        <v>-0.65603</v>
+      </c>
+      <c r="S39" s="10">
+        <v>0.98</v>
+      </c>
+      <c r="T39" s="10">
+        <v>0.88</v>
+      </c>
+      <c r="U39" s="10">
+        <v>-0.10183</v>
+      </c>
+      <c r="V39" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="W39" s="7">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C40" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="7">
+        <v>-7.92</v>
+      </c>
+      <c r="E40" s="9">
+        <v>-9.82</v>
+      </c>
+      <c r="F40" s="5">
+        <v>-1.9097200000000001</v>
+      </c>
+      <c r="G40" s="5">
+        <v>0.24127000000000001</v>
+      </c>
+      <c r="H40" s="5">
+        <v>0.77</v>
+      </c>
+      <c r="I40" s="5">
+        <v>0.69</v>
+      </c>
+      <c r="J40" s="5">
+        <v>-9.894E-2</v>
+      </c>
+      <c r="K40" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="L40" s="2">
+        <v>1</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O40" s="7">
+        <v>-7.78</v>
+      </c>
+      <c r="P40" s="9">
+        <v>-11.73</v>
+      </c>
+      <c r="Q40" s="10">
+        <v>-3.9555899999999999</v>
+      </c>
+      <c r="R40" s="10">
+        <v>0.50866</v>
+      </c>
+      <c r="S40" s="10">
+        <v>0.98</v>
+      </c>
+      <c r="T40" s="10">
+        <v>0.93</v>
+      </c>
+      <c r="U40" s="10">
+        <v>-4.5859999999999998E-2</v>
+      </c>
+      <c r="V40" s="7">
         <v>0.04</v>
       </c>
-      <c r="Q32" s="10">
+      <c r="W40" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C41" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="7">
+        <v>5.87</v>
+      </c>
+      <c r="E41" s="9">
+        <v>6.02</v>
+      </c>
+      <c r="F41" s="5">
+        <v>0.14910000000000001</v>
+      </c>
+      <c r="G41" s="5">
+        <v>2.5409999999999999E-2</v>
+      </c>
+      <c r="H41" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="I41" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="J41" s="5">
+        <v>4.419E-2</v>
+      </c>
+      <c r="K41" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="L41" s="2">
+        <v>1</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O41" s="7">
+        <v>5.86</v>
+      </c>
+      <c r="P41" s="9">
+        <v>5.99</v>
+      </c>
+      <c r="Q41" s="10">
+        <v>0.12862999999999999</v>
+      </c>
+      <c r="R41" s="10">
+        <v>2.1930000000000002E-2</v>
+      </c>
+      <c r="S41" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="T41" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="U41" s="10">
+        <v>0.10811</v>
+      </c>
+      <c r="V41" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="W41" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C42" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="7">
+        <v>0.03</v>
+      </c>
+      <c r="E42" s="9">
+        <v>0.02</v>
+      </c>
+      <c r="F42" s="5">
+        <v>-4.0499999999999998E-3</v>
+      </c>
+      <c r="G42" s="5">
+        <v>-0.14241999999999999</v>
+      </c>
+      <c r="H42" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="I42" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="J42" s="5">
+        <v>-4.9259999999999998E-2</v>
+      </c>
+      <c r="K42" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="L42" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O42" s="7">
+        <v>0.03</v>
+      </c>
+      <c r="P42" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="Q42" s="10">
         <v>8.4200000000000004E-3</v>
       </c>
-      <c r="R32" s="10">
+      <c r="R42" s="10">
         <v>0.26218000000000002</v>
       </c>
-      <c r="S32" s="10">
+      <c r="S42" s="10">
         <v>0.03</v>
       </c>
-      <c r="T32" s="10">
+      <c r="T42" s="10">
         <v>0.02</v>
       </c>
-      <c r="U32" s="10">
+      <c r="U42" s="10">
         <v>-8.0159999999999995E-2</v>
       </c>
-      <c r="V32" s="7">
+      <c r="V42" s="7">
         <v>0.92</v>
       </c>
-      <c r="W32" s="7">
+      <c r="W42" s="7">
         <v>0.33</v>
       </c>
     </row>
-    <row r="33" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-    </row>
-    <row r="34" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="11"/>
-      <c r="M34" s="11"/>
+    <row r="43" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11"/>
+    </row>
+    <row r="44" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="C24:L24"/>
-    <mergeCell ref="N24:W24"/>
+  <mergeCells count="10">
+    <mergeCell ref="C34:L34"/>
+    <mergeCell ref="N34:W34"/>
     <mergeCell ref="N14:W14"/>
     <mergeCell ref="C14:L14"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="N4:W4"/>
     <mergeCell ref="C4:L4"/>
+    <mergeCell ref="C24:L24"/>
+    <mergeCell ref="N24:W24"/>
   </mergeCells>
   <conditionalFormatting sqref="K6:K12">
-    <cfRule type="cellIs" dxfId="88" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="79" priority="31" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="32" operator="equal">
       <formula>0.95</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="13" operator="between">
+    <cfRule type="cellIs" dxfId="77" priority="33" operator="between">
       <formula>0.5</formula>
       <formula>0.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="14" operator="between">
+    <cfRule type="cellIs" dxfId="76" priority="34" operator="between">
       <formula>0.9</formula>
       <formula>0.9499999</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="75" priority="35" operator="greaterThan">
       <formula>0.95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16:K22">
-    <cfRule type="cellIs" dxfId="83" priority="31" operator="lessThan">
+    <cfRule type="cellIs" dxfId="74" priority="51" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="52" operator="equal">
       <formula>0.95</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="33" operator="between">
+    <cfRule type="cellIs" dxfId="72" priority="53" operator="between">
       <formula>0.5</formula>
       <formula>0.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="34" operator="between">
+    <cfRule type="cellIs" dxfId="71" priority="54" operator="between">
       <formula>0.9</formula>
       <formula>0.9499999</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="70" priority="55" operator="greaterThan">
+      <formula>0.95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K36:K42">
+    <cfRule type="cellIs" dxfId="69" priority="84" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="85" operator="equal">
+      <formula>0.95</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="86" operator="between">
+      <formula>0.5</formula>
+      <formula>0.9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="87" operator="between">
+      <formula>0.9</formula>
+      <formula>0.9499999</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="88" operator="greaterThan">
+      <formula>0.95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V6:V12">
+    <cfRule type="cellIs" dxfId="64" priority="21" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="22" operator="equal">
+      <formula>0.95</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="23" operator="between">
+      <formula>0.5</formula>
+      <formula>0.9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="24" operator="between">
+      <formula>0.9</formula>
+      <formula>0.9499999</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="25" operator="greaterThan">
+      <formula>0.95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V16:V22">
+    <cfRule type="cellIs" dxfId="59" priority="46" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="47" operator="equal">
+      <formula>0.95</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="48" operator="between">
+      <formula>0.5</formula>
+      <formula>0.9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="49" operator="between">
+      <formula>0.9</formula>
+      <formula>0.9499999</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="50" operator="greaterThan">
+      <formula>0.95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V36:V42">
+    <cfRule type="cellIs" dxfId="54" priority="79" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="80" operator="equal">
+      <formula>0.95</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="81" operator="between">
+      <formula>0.5</formula>
+      <formula>0.9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="82" operator="between">
+      <formula>0.9</formula>
+      <formula>0.9499999</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="83" operator="greaterThan">
       <formula>0.95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26:K32">
-    <cfRule type="cellIs" dxfId="78" priority="64" operator="lessThan">
+    <cfRule type="cellIs" dxfId="49" priority="1" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="2" operator="equal">
       <formula>0.95</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="66" operator="between">
+    <cfRule type="cellIs" dxfId="47" priority="3" operator="between">
       <formula>0.5</formula>
       <formula>0.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="67" operator="between">
+    <cfRule type="cellIs" dxfId="46" priority="4" operator="between">
       <formula>0.9</formula>
       <formula>0.9499999</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="68" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="5" operator="greaterThan">
       <formula>0.95</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V16:V22">
-    <cfRule type="cellIs" dxfId="68" priority="26" operator="lessThan">
+  <conditionalFormatting sqref="V26:V32">
+    <cfRule type="cellIs" dxfId="44" priority="6" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="7" operator="equal">
       <formula>0.95</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="28" operator="between">
+    <cfRule type="cellIs" dxfId="42" priority="8" operator="between">
       <formula>0.5</formula>
       <formula>0.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="29" operator="between">
+    <cfRule type="cellIs" dxfId="41" priority="9" operator="between">
       <formula>0.9</formula>
       <formula>0.9499999</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="30" operator="greaterThan">
-      <formula>0.95</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V26:V32">
-    <cfRule type="cellIs" dxfId="63" priority="59" operator="lessThan">
-      <formula>0.5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="60" operator="equal">
-      <formula>0.95</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="61" operator="between">
-      <formula>0.5</formula>
-      <formula>0.9</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="62" operator="between">
-      <formula>0.9</formula>
-      <formula>0.9499999</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="63" operator="greaterThan">
-      <formula>0.95</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V6:V12">
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="lessThan">
-      <formula>0.5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
-      <formula>0.95</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="3" operator="between">
-      <formula>0.5</formula>
-      <formula>0.9</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="4" operator="between">
-      <formula>0.9</formula>
-      <formula>0.9499999</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="10" operator="greaterThan">
       <formula>0.95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2983,10 +3488,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6665CD2B-B7E3-4BBB-A6EA-3E83EE4922E0}">
-  <dimension ref="A1:AV34"/>
+  <dimension ref="A1:AV44"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Y28" sqref="Y28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4127,7 +4632,7 @@
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="C24" s="13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
@@ -4139,7 +4644,7 @@
       <c r="K24" s="13"/>
       <c r="L24" s="13"/>
       <c r="N24" s="13" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="O24" s="13"/>
       <c r="P24" s="13"/>
@@ -4221,28 +4726,28 @@
         <v>107.08</v>
       </c>
       <c r="E26" s="9">
-        <v>101.63</v>
-      </c>
-      <c r="F26" s="5">
-        <v>-5.4487899999999998</v>
-      </c>
-      <c r="G26" s="5">
-        <v>-5.0889999999999998E-2</v>
-      </c>
-      <c r="H26" s="5">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="I26" s="5">
-        <v>2.0699999999999998</v>
-      </c>
-      <c r="J26" s="5">
-        <v>-9.1909000000000005E-2</v>
+        <v>106.64422999999999</v>
+      </c>
+      <c r="F26" s="10">
+        <v>-0.43318000000000001</v>
+      </c>
+      <c r="G26" s="10">
+        <v>-4.0499999999999998E-3</v>
+      </c>
+      <c r="H26" s="10">
+        <v>3.3864969999999999</v>
+      </c>
+      <c r="I26" s="10">
+        <v>3.196968</v>
+      </c>
+      <c r="J26" s="10">
+        <v>-5.5969999999999999E-2</v>
       </c>
       <c r="K26" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="L26" s="2">
-        <v>1</v>
+        <v>0.93</v>
+      </c>
+      <c r="L26" s="7">
+        <v>0</v>
       </c>
       <c r="N26" s="1" t="s">
         <v>0</v>
@@ -4251,28 +4756,28 @@
         <v>106.81</v>
       </c>
       <c r="P26" s="9">
-        <v>97.82</v>
-      </c>
-      <c r="Q26" s="5">
-        <v>-8.9958600000000004</v>
-      </c>
-      <c r="R26" s="5">
-        <v>-8.4220000000000003E-2</v>
-      </c>
-      <c r="S26" s="5">
-        <v>3.58</v>
-      </c>
-      <c r="T26" s="5">
-        <v>3.25</v>
-      </c>
-      <c r="U26" s="5">
-        <v>-9.3140000000000001E-2</v>
+        <v>107.222015</v>
+      </c>
+      <c r="Q26" s="10">
+        <v>0.40955999999999998</v>
+      </c>
+      <c r="R26" s="10">
+        <v>3.8300000000000001E-3</v>
+      </c>
+      <c r="S26" s="10">
+        <v>4.5790819999999997</v>
+      </c>
+      <c r="T26" s="10">
+        <v>4.2662269999999998</v>
+      </c>
+      <c r="U26" s="10">
+        <v>-6.8320000000000006E-2</v>
       </c>
       <c r="V26" s="7">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="W26" s="2">
-        <v>1</v>
+        <v>0.94</v>
+      </c>
+      <c r="W26" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
@@ -4283,28 +4788,28 @@
         <v>-4.7699999999999996</v>
       </c>
       <c r="E27" s="9">
-        <v>-3.9</v>
-      </c>
-      <c r="F27" s="5">
-        <v>0.86375999999999997</v>
-      </c>
-      <c r="G27" s="5">
-        <v>-0.18113000000000001</v>
-      </c>
-      <c r="H27" s="5">
-        <v>0.85</v>
-      </c>
-      <c r="I27" s="5">
-        <v>0.84</v>
-      </c>
-      <c r="J27" s="5">
-        <v>-1.3242E-2</v>
+        <v>-3.6062850000000002</v>
+      </c>
+      <c r="F27" s="10">
+        <v>1.1623600000000001</v>
+      </c>
+      <c r="G27" s="10">
+        <v>-0.24374999999999999</v>
+      </c>
+      <c r="H27" s="10">
+        <v>1.497196</v>
+      </c>
+      <c r="I27" s="10">
+        <v>1.439076</v>
+      </c>
+      <c r="J27" s="10">
+        <v>-3.882E-2</v>
       </c>
       <c r="K27" s="7">
-        <v>0.82</v>
-      </c>
-      <c r="L27" s="2">
-        <v>0.98</v>
+        <v>0.9</v>
+      </c>
+      <c r="L27" s="7">
+        <v>0</v>
       </c>
       <c r="N27" s="1" t="s">
         <v>11</v>
@@ -4313,28 +4818,28 @@
         <v>-4.8</v>
       </c>
       <c r="P27" s="9">
-        <v>-4.16</v>
-      </c>
-      <c r="Q27" s="5">
-        <v>0.64359</v>
-      </c>
-      <c r="R27" s="5">
-        <v>-0.1341</v>
-      </c>
-      <c r="S27" s="5">
-        <v>1.31</v>
-      </c>
-      <c r="T27" s="5">
-        <v>1.26</v>
-      </c>
-      <c r="U27" s="5">
-        <v>-4.1300000000000003E-2</v>
+        <v>-3.6082450000000001</v>
+      </c>
+      <c r="Q27" s="10">
+        <v>1.1910400000000001</v>
+      </c>
+      <c r="R27" s="10">
+        <v>-0.24817</v>
+      </c>
+      <c r="S27" s="10">
+        <v>1.8769929999999999</v>
+      </c>
+      <c r="T27" s="10">
+        <v>1.764634</v>
+      </c>
+      <c r="U27" s="10">
+        <v>-5.9859999999999997E-2</v>
       </c>
       <c r="V27" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="W27" s="2">
-        <v>0.85</v>
+        <v>0.92</v>
+      </c>
+      <c r="W27" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
@@ -4345,28 +4850,28 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="E28" s="9">
-        <v>10.59</v>
-      </c>
-      <c r="F28" s="5">
-        <v>1.89225</v>
-      </c>
-      <c r="G28" s="5">
-        <v>0.21758</v>
-      </c>
-      <c r="H28" s="5">
-        <v>0.51</v>
-      </c>
-      <c r="I28" s="5">
-        <v>0.49</v>
-      </c>
-      <c r="J28" s="5">
-        <v>-4.3602000000000002E-2</v>
+        <v>8.6159859999999995</v>
+      </c>
+      <c r="F28" s="10">
+        <v>-8.0710000000000004E-2</v>
+      </c>
+      <c r="G28" s="10">
+        <v>-9.2800000000000001E-3</v>
+      </c>
+      <c r="H28" s="10">
+        <v>0.62467600000000001</v>
+      </c>
+      <c r="I28" s="10">
+        <v>0.61796700000000004</v>
+      </c>
+      <c r="J28" s="10">
+        <v>-1.074E-2</v>
       </c>
       <c r="K28" s="7">
-        <v>0.02</v>
-      </c>
-      <c r="L28" s="2">
-        <v>1</v>
+        <v>0.95</v>
+      </c>
+      <c r="L28" s="7">
+        <v>0</v>
       </c>
       <c r="N28" s="1" t="s">
         <v>12</v>
@@ -4375,28 +4880,28 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="P28" s="9">
-        <v>12.85</v>
-      </c>
-      <c r="Q28" s="5">
-        <v>4.1436500000000001</v>
-      </c>
-      <c r="R28" s="5">
-        <v>0.47616000000000003</v>
-      </c>
-      <c r="S28" s="5">
-        <v>0.7</v>
-      </c>
-      <c r="T28" s="5">
-        <v>0.68</v>
-      </c>
-      <c r="U28" s="5">
-        <v>-2.9649999999999999E-2</v>
+        <v>8.6706769999999995</v>
+      </c>
+      <c r="Q28" s="10">
+        <v>-3.1530000000000002E-2</v>
+      </c>
+      <c r="R28" s="10">
+        <v>-3.62E-3</v>
+      </c>
+      <c r="S28" s="10">
+        <v>0.79806299999999997</v>
+      </c>
+      <c r="T28" s="10">
+        <v>0.74026099999999995</v>
+      </c>
+      <c r="U28" s="10">
+        <v>-7.2429999999999994E-2</v>
       </c>
       <c r="V28" s="7">
-        <v>0</v>
-      </c>
-      <c r="W28" s="2">
-        <v>1</v>
+        <v>0.93</v>
+      </c>
+      <c r="W28" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
@@ -4407,28 +4912,28 @@
         <v>-1.61</v>
       </c>
       <c r="E29" s="9">
-        <v>-1</v>
-      </c>
-      <c r="F29" s="5">
-        <v>0.61197999999999997</v>
-      </c>
-      <c r="G29" s="5">
-        <v>-0.38003999999999999</v>
-      </c>
-      <c r="H29" s="5">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="I29" s="5">
-        <v>0.52</v>
-      </c>
-      <c r="J29" s="5">
-        <v>-5.4073999999999997E-2</v>
+        <v>-1.8730770000000001</v>
+      </c>
+      <c r="F29" s="10">
+        <v>-0.26278000000000001</v>
+      </c>
+      <c r="G29" s="10">
+        <v>0.16319</v>
+      </c>
+      <c r="H29" s="10">
+        <v>0.86055300000000001</v>
+      </c>
+      <c r="I29" s="10">
+        <v>0.76639000000000002</v>
+      </c>
+      <c r="J29" s="10">
+        <v>-0.10942</v>
       </c>
       <c r="K29" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="L29" s="2">
-        <v>0.36</v>
+        <v>0.89</v>
+      </c>
+      <c r="L29" s="7">
+        <v>0</v>
       </c>
       <c r="N29" s="1" t="s">
         <v>13</v>
@@ -4437,28 +4942,28 @@
         <v>-1.58</v>
       </c>
       <c r="P29" s="9">
-        <v>-0.56999999999999995</v>
-      </c>
-      <c r="Q29" s="5">
-        <v>1.0102899999999999</v>
-      </c>
-      <c r="R29" s="5">
-        <v>-0.63917000000000002</v>
-      </c>
-      <c r="S29" s="5">
-        <v>0.88</v>
-      </c>
-      <c r="T29" s="5">
-        <v>0.84</v>
-      </c>
-      <c r="U29" s="5">
-        <v>-4.5190000000000001E-2</v>
+        <v>-2.1472920000000002</v>
+      </c>
+      <c r="Q29" s="10">
+        <v>-0.56667000000000001</v>
+      </c>
+      <c r="R29" s="10">
+        <v>0.35851</v>
+      </c>
+      <c r="S29" s="10">
+        <v>1.1460129999999999</v>
+      </c>
+      <c r="T29" s="10">
+        <v>1.023026</v>
+      </c>
+      <c r="U29" s="10">
+        <v>-0.10732</v>
       </c>
       <c r="V29" s="7">
-        <v>0.71</v>
-      </c>
-      <c r="W29" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>0.89</v>
+      </c>
+      <c r="W29" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
@@ -4469,28 +4974,28 @@
         <v>-7.92</v>
       </c>
       <c r="E30" s="9">
-        <v>-10.08</v>
-      </c>
-      <c r="F30" s="5">
-        <v>-2.1660599999999999</v>
-      </c>
-      <c r="G30" s="5">
-        <v>0.27366000000000001</v>
-      </c>
-      <c r="H30" s="5">
-        <v>0.72</v>
-      </c>
-      <c r="I30" s="5">
-        <v>0.66</v>
-      </c>
-      <c r="J30" s="5">
-        <v>-7.6568999999999998E-2</v>
+        <v>-8.1076789999999992</v>
+      </c>
+      <c r="F30" s="10">
+        <v>-0.1925</v>
+      </c>
+      <c r="G30" s="10">
+        <v>2.4320000000000001E-2</v>
+      </c>
+      <c r="H30" s="10">
+        <v>0.86592899999999995</v>
+      </c>
+      <c r="I30" s="10">
+        <v>0.81638900000000003</v>
+      </c>
+      <c r="J30" s="10">
+        <v>-5.7209999999999997E-2</v>
       </c>
       <c r="K30" s="7">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="L30" s="2">
-        <v>1</v>
+        <v>0.94</v>
+      </c>
+      <c r="L30" s="7">
+        <v>0</v>
       </c>
       <c r="N30" s="1" t="s">
         <v>14</v>
@@ -4499,28 +5004,28 @@
         <v>-7.78</v>
       </c>
       <c r="P30" s="9">
-        <v>-11.97</v>
-      </c>
-      <c r="Q30" s="5">
-        <v>-4.1970999999999998</v>
-      </c>
-      <c r="R30" s="5">
-        <v>0.53971999999999998</v>
-      </c>
-      <c r="S30" s="5">
-        <v>0.96</v>
-      </c>
-      <c r="T30" s="5">
-        <v>0.92</v>
-      </c>
-      <c r="U30" s="5">
-        <v>-4.6870000000000002E-2</v>
+        <v>-8.0386179999999996</v>
+      </c>
+      <c r="Q30" s="10">
+        <v>-0.26218999999999998</v>
+      </c>
+      <c r="R30" s="10">
+        <v>3.372E-2</v>
+      </c>
+      <c r="S30" s="10">
+        <v>1.0560529999999999</v>
+      </c>
+      <c r="T30" s="10">
+        <v>0.98724699999999999</v>
+      </c>
+      <c r="U30" s="10">
+        <v>-6.515E-2</v>
       </c>
       <c r="V30" s="7">
-        <v>0.02</v>
-      </c>
-      <c r="W30" s="2">
-        <v>1</v>
+        <v>0.97</v>
+      </c>
+      <c r="W30" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
@@ -4531,28 +5036,28 @@
         <v>5.87</v>
       </c>
       <c r="E31" s="9">
-        <v>5.97</v>
-      </c>
-      <c r="F31" s="5">
-        <v>9.8369999999999999E-2</v>
-      </c>
-      <c r="G31" s="5">
-        <v>1.6760000000000001E-2</v>
-      </c>
-      <c r="H31" s="5">
-        <v>0.04</v>
-      </c>
-      <c r="I31" s="5">
-        <v>0.04</v>
-      </c>
-      <c r="J31" s="5">
-        <v>7.9797999999999994E-2</v>
+        <v>5.8871440000000002</v>
+      </c>
+      <c r="F31" s="10">
+        <v>1.9E-2</v>
+      </c>
+      <c r="G31" s="10">
+        <v>3.2399999999999998E-3</v>
+      </c>
+      <c r="H31" s="10">
+        <v>5.4842000000000002E-2</v>
+      </c>
+      <c r="I31" s="10">
+        <v>6.7028000000000004E-2</v>
+      </c>
+      <c r="J31" s="10">
+        <v>0.22219</v>
       </c>
       <c r="K31" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="L31" s="2">
-        <v>1</v>
+        <v>0.97</v>
+      </c>
+      <c r="L31" s="7">
+        <v>0</v>
       </c>
       <c r="N31" s="1" t="s">
         <v>15</v>
@@ -4561,28 +5066,28 @@
         <v>5.86</v>
       </c>
       <c r="P31" s="9">
-        <v>5.99</v>
-      </c>
-      <c r="Q31" s="5">
-        <v>0.12895000000000001</v>
-      </c>
-      <c r="R31" s="5">
-        <v>2.1989999999999999E-2</v>
-      </c>
-      <c r="S31" s="5">
-        <v>0.03</v>
-      </c>
-      <c r="T31" s="5">
-        <v>0.03</v>
-      </c>
-      <c r="U31" s="5">
-        <v>0.12066</v>
+        <v>5.8675949999999997</v>
+      </c>
+      <c r="Q31" s="10">
+        <v>3.1800000000000001E-3</v>
+      </c>
+      <c r="R31" s="10">
+        <v>5.4000000000000001E-4</v>
+      </c>
+      <c r="S31" s="10">
+        <v>6.4696000000000004E-2</v>
+      </c>
+      <c r="T31" s="10">
+        <v>7.8047000000000005E-2</v>
+      </c>
+      <c r="U31" s="10">
+        <v>0.20637</v>
       </c>
       <c r="V31" s="7">
-        <v>0.02</v>
-      </c>
-      <c r="W31" s="2">
-        <v>1</v>
+        <v>0.98</v>
+      </c>
+      <c r="W31" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
@@ -4593,28 +5098,28 @@
         <v>0.03</v>
       </c>
       <c r="E32" s="9">
-        <v>0.03</v>
-      </c>
-      <c r="F32" s="5">
-        <v>-6.8000000000000005E-4</v>
-      </c>
-      <c r="G32" s="5">
-        <v>-2.4039999999999999E-2</v>
-      </c>
-      <c r="H32" s="5">
-        <v>0.03</v>
-      </c>
-      <c r="I32" s="5">
-        <v>0.02</v>
-      </c>
-      <c r="J32" s="5">
-        <v>-1.5807999999999999E-2</v>
+        <v>2.9242000000000001E-2</v>
+      </c>
+      <c r="F32" s="10">
+        <v>8.3000000000000001E-4</v>
+      </c>
+      <c r="G32" s="10">
+        <v>2.9059999999999999E-2</v>
+      </c>
+      <c r="H32" s="10">
+        <v>4.7524999999999998E-2</v>
+      </c>
+      <c r="I32" s="10">
+        <v>5.6641999999999998E-2</v>
+      </c>
+      <c r="J32" s="10">
+        <v>0.19184999999999999</v>
       </c>
       <c r="K32" s="7">
-        <v>0.95</v>
-      </c>
-      <c r="L32" s="2">
-        <v>0.17</v>
+        <v>1</v>
+      </c>
+      <c r="L32" s="7">
+        <v>0</v>
       </c>
       <c r="N32" s="1" t="s">
         <v>16</v>
@@ -4623,163 +5128,725 @@
         <v>0.03</v>
       </c>
       <c r="P32" s="9">
+        <v>4.8389000000000001E-2</v>
+      </c>
+      <c r="Q32" s="10">
+        <v>1.6279999999999999E-2</v>
+      </c>
+      <c r="R32" s="10">
+        <v>0.50705999999999996</v>
+      </c>
+      <c r="S32" s="10">
+        <v>5.8416999999999997E-2</v>
+      </c>
+      <c r="T32" s="10">
+        <v>6.9318000000000005E-2</v>
+      </c>
+      <c r="U32" s="10">
+        <v>0.18659999999999999</v>
+      </c>
+      <c r="V32" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="W32" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C34" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="N34" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="O34" s="13"/>
+      <c r="P34" s="13"/>
+      <c r="Q34" s="13"/>
+      <c r="R34" s="13"/>
+      <c r="S34" s="13"/>
+      <c r="T34" s="13"/>
+      <c r="U34" s="13"/>
+      <c r="V34" s="13"/>
+      <c r="W34" s="13"/>
+    </row>
+    <row r="35" spans="3:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="C35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L35" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O35" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P35" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="R35" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="T35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="U35" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="V35" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W35" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C36" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" s="7">
+        <v>107.08</v>
+      </c>
+      <c r="E36" s="9">
+        <v>101.63</v>
+      </c>
+      <c r="F36" s="5">
+        <v>-5.4487899999999998</v>
+      </c>
+      <c r="G36" s="5">
+        <v>-5.0889999999999998E-2</v>
+      </c>
+      <c r="H36" s="5">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="I36" s="5">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="J36" s="5">
+        <v>-9.1909000000000005E-2</v>
+      </c>
+      <c r="K36" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="L36" s="2">
+        <v>1</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O36" s="7">
+        <v>106.81</v>
+      </c>
+      <c r="P36" s="9">
+        <v>97.82</v>
+      </c>
+      <c r="Q36" s="5">
+        <v>-8.9958600000000004</v>
+      </c>
+      <c r="R36" s="5">
+        <v>-8.4220000000000003E-2</v>
+      </c>
+      <c r="S36" s="5">
+        <v>3.58</v>
+      </c>
+      <c r="T36" s="5">
+        <v>3.25</v>
+      </c>
+      <c r="U36" s="5">
+        <v>-9.3140000000000001E-2</v>
+      </c>
+      <c r="V36" s="7">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="W36" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C37" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="7">
+        <v>-4.7699999999999996</v>
+      </c>
+      <c r="E37" s="9">
+        <v>-3.9</v>
+      </c>
+      <c r="F37" s="5">
+        <v>0.86375999999999997</v>
+      </c>
+      <c r="G37" s="5">
+        <v>-0.18113000000000001</v>
+      </c>
+      <c r="H37" s="5">
+        <v>0.85</v>
+      </c>
+      <c r="I37" s="5">
+        <v>0.84</v>
+      </c>
+      <c r="J37" s="5">
+        <v>-1.3242E-2</v>
+      </c>
+      <c r="K37" s="7">
+        <v>0.82</v>
+      </c>
+      <c r="L37" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O37" s="7">
+        <v>-4.8</v>
+      </c>
+      <c r="P37" s="9">
+        <v>-4.16</v>
+      </c>
+      <c r="Q37" s="5">
+        <v>0.64359</v>
+      </c>
+      <c r="R37" s="5">
+        <v>-0.1341</v>
+      </c>
+      <c r="S37" s="5">
+        <v>1.31</v>
+      </c>
+      <c r="T37" s="5">
+        <v>1.26</v>
+      </c>
+      <c r="U37" s="5">
+        <v>-4.1300000000000003E-2</v>
+      </c>
+      <c r="V37" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="W37" s="2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="38" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C38" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="7">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="E38" s="9">
+        <v>10.59</v>
+      </c>
+      <c r="F38" s="5">
+        <v>1.89225</v>
+      </c>
+      <c r="G38" s="5">
+        <v>0.21758</v>
+      </c>
+      <c r="H38" s="5">
+        <v>0.51</v>
+      </c>
+      <c r="I38" s="5">
+        <v>0.49</v>
+      </c>
+      <c r="J38" s="5">
+        <v>-4.3602000000000002E-2</v>
+      </c>
+      <c r="K38" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="L38" s="2">
+        <v>1</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O38" s="7">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="P38" s="9">
+        <v>12.85</v>
+      </c>
+      <c r="Q38" s="5">
+        <v>4.1436500000000001</v>
+      </c>
+      <c r="R38" s="5">
+        <v>0.47616000000000003</v>
+      </c>
+      <c r="S38" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="T38" s="5">
+        <v>0.68</v>
+      </c>
+      <c r="U38" s="5">
+        <v>-2.9649999999999999E-2</v>
+      </c>
+      <c r="V38" s="7">
+        <v>0</v>
+      </c>
+      <c r="W38" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C39" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="7">
+        <v>-1.61</v>
+      </c>
+      <c r="E39" s="9">
+        <v>-1</v>
+      </c>
+      <c r="F39" s="5">
+        <v>0.61197999999999997</v>
+      </c>
+      <c r="G39" s="5">
+        <v>-0.38003999999999999</v>
+      </c>
+      <c r="H39" s="5">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I39" s="5">
+        <v>0.52</v>
+      </c>
+      <c r="J39" s="5">
+        <v>-5.4073999999999997E-2</v>
+      </c>
+      <c r="K39" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="L39" s="2">
+        <v>0.36</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O39" s="7">
+        <v>-1.58</v>
+      </c>
+      <c r="P39" s="9">
+        <v>-0.56999999999999995</v>
+      </c>
+      <c r="Q39" s="5">
+        <v>1.0102899999999999</v>
+      </c>
+      <c r="R39" s="5">
+        <v>-0.63917000000000002</v>
+      </c>
+      <c r="S39" s="5">
+        <v>0.88</v>
+      </c>
+      <c r="T39" s="5">
+        <v>0.84</v>
+      </c>
+      <c r="U39" s="5">
+        <v>-4.5190000000000001E-2</v>
+      </c>
+      <c r="V39" s="7">
+        <v>0.71</v>
+      </c>
+      <c r="W39" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C40" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="7">
+        <v>-7.92</v>
+      </c>
+      <c r="E40" s="9">
+        <v>-10.08</v>
+      </c>
+      <c r="F40" s="5">
+        <v>-2.1660599999999999</v>
+      </c>
+      <c r="G40" s="5">
+        <v>0.27366000000000001</v>
+      </c>
+      <c r="H40" s="5">
+        <v>0.72</v>
+      </c>
+      <c r="I40" s="5">
+        <v>0.66</v>
+      </c>
+      <c r="J40" s="5">
+        <v>-7.6568999999999998E-2</v>
+      </c>
+      <c r="K40" s="7">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="L40" s="2">
+        <v>1</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O40" s="7">
+        <v>-7.78</v>
+      </c>
+      <c r="P40" s="9">
+        <v>-11.97</v>
+      </c>
+      <c r="Q40" s="5">
+        <v>-4.1970999999999998</v>
+      </c>
+      <c r="R40" s="5">
+        <v>0.53971999999999998</v>
+      </c>
+      <c r="S40" s="5">
+        <v>0.96</v>
+      </c>
+      <c r="T40" s="5">
+        <v>0.92</v>
+      </c>
+      <c r="U40" s="5">
+        <v>-4.6870000000000002E-2</v>
+      </c>
+      <c r="V40" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="W40" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C41" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="7">
+        <v>5.87</v>
+      </c>
+      <c r="E41" s="9">
+        <v>5.97</v>
+      </c>
+      <c r="F41" s="5">
+        <v>9.8369999999999999E-2</v>
+      </c>
+      <c r="G41" s="5">
+        <v>1.6760000000000001E-2</v>
+      </c>
+      <c r="H41" s="5">
         <v>0.04</v>
       </c>
-      <c r="Q32" s="5">
+      <c r="I41" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="J41" s="5">
+        <v>7.9797999999999994E-2</v>
+      </c>
+      <c r="K41" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="L41" s="2">
+        <v>1</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O41" s="7">
+        <v>5.86</v>
+      </c>
+      <c r="P41" s="9">
+        <v>5.99</v>
+      </c>
+      <c r="Q41" s="5">
+        <v>0.12895000000000001</v>
+      </c>
+      <c r="R41" s="5">
+        <v>2.1989999999999999E-2</v>
+      </c>
+      <c r="S41" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="T41" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="U41" s="5">
+        <v>0.12066</v>
+      </c>
+      <c r="V41" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="W41" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C42" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="7">
+        <v>0.03</v>
+      </c>
+      <c r="E42" s="9">
+        <v>0.03</v>
+      </c>
+      <c r="F42" s="5">
+        <v>-6.8000000000000005E-4</v>
+      </c>
+      <c r="G42" s="5">
+        <v>-2.4039999999999999E-2</v>
+      </c>
+      <c r="H42" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="I42" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="J42" s="5">
+        <v>-1.5807999999999999E-2</v>
+      </c>
+      <c r="K42" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="L42" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O42" s="7">
+        <v>0.03</v>
+      </c>
+      <c r="P42" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="Q42" s="5">
         <v>8.6800000000000002E-3</v>
       </c>
-      <c r="R32" s="5">
+      <c r="R42" s="5">
         <v>0.27022000000000002</v>
       </c>
-      <c r="S32" s="5">
+      <c r="S42" s="5">
         <v>0.02</v>
       </c>
-      <c r="T32" s="5">
+      <c r="T42" s="5">
         <v>0.02</v>
       </c>
-      <c r="U32" s="5">
+      <c r="U42" s="5">
         <v>-5.6739999999999999E-2</v>
       </c>
-      <c r="V32" s="7">
+      <c r="V42" s="7">
         <v>0.93</v>
       </c>
-      <c r="W32" s="2">
+      <c r="W42" s="2">
         <v>0.38</v>
       </c>
     </row>
-    <row r="33" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-    </row>
-    <row r="34" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="11"/>
-      <c r="M34" s="11"/>
+    <row r="43" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11"/>
+    </row>
+    <row r="44" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="C24:L24"/>
-    <mergeCell ref="N24:W24"/>
+  <mergeCells count="10">
+    <mergeCell ref="C34:L34"/>
+    <mergeCell ref="N34:W34"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="C4:L4"/>
     <mergeCell ref="N4:W4"/>
     <mergeCell ref="C14:L14"/>
     <mergeCell ref="N14:W14"/>
+    <mergeCell ref="C24:L24"/>
+    <mergeCell ref="N24:W24"/>
   </mergeCells>
-  <conditionalFormatting sqref="K26:K32">
-    <cfRule type="cellIs" dxfId="48" priority="45" operator="lessThan">
+  <conditionalFormatting sqref="K6:K12">
+    <cfRule type="cellIs" dxfId="39" priority="26" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="27" operator="equal">
       <formula>0.95</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="47" operator="between">
+    <cfRule type="cellIs" dxfId="37" priority="28" operator="between">
       <formula>0.5</formula>
       <formula>0.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="48" operator="between">
+    <cfRule type="cellIs" dxfId="36" priority="29" operator="between">
       <formula>0.9</formula>
       <formula>0.9499999</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="49" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="30" operator="greaterThan">
+      <formula>0.95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16:K22">
+    <cfRule type="cellIs" dxfId="34" priority="21" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="22" operator="equal">
+      <formula>0.95</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="23" operator="between">
+      <formula>0.5</formula>
+      <formula>0.9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="24" operator="between">
+      <formula>0.9</formula>
+      <formula>0.9499999</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="25" operator="greaterThan">
+      <formula>0.95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K36:K42">
+    <cfRule type="cellIs" dxfId="29" priority="60" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="61" operator="equal">
+      <formula>0.95</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="62" operator="between">
+      <formula>0.5</formula>
+      <formula>0.9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="63" operator="between">
+      <formula>0.9</formula>
+      <formula>0.9499999</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="64" operator="greaterThan">
+      <formula>0.95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V6:V12">
+    <cfRule type="cellIs" dxfId="24" priority="31" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="32" operator="equal">
+      <formula>0.95</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="33" operator="between">
+      <formula>0.5</formula>
+      <formula>0.9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="34" operator="between">
+      <formula>0.9</formula>
+      <formula>0.9499999</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="35" operator="greaterThan">
+      <formula>0.95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V16:V22">
+    <cfRule type="cellIs" dxfId="19" priority="16" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
+      <formula>0.95</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="between">
+      <formula>0.5</formula>
+      <formula>0.9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="19" operator="between">
+      <formula>0.9</formula>
+      <formula>0.9499999</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="20" operator="greaterThan">
+      <formula>0.95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V36:V42">
+    <cfRule type="cellIs" dxfId="14" priority="46" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="47" operator="equal">
+      <formula>0.95</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="48" operator="between">
+      <formula>0.5</formula>
+      <formula>0.9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="49" operator="between">
+      <formula>0.9</formula>
+      <formula>0.9499999</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="50" operator="greaterThan">
       <formula>0.95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V26:V32">
-    <cfRule type="cellIs" dxfId="34" priority="31" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
       <formula>0.95</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="33" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="13" operator="between">
       <formula>0.5</formula>
       <formula>0.9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="34" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="14" operator="between">
       <formula>0.9</formula>
       <formula>0.9499999</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="15" operator="greaterThan">
       <formula>0.95</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V6:V12">
-    <cfRule type="cellIs" dxfId="24" priority="16" operator="lessThan">
-      <formula>0.5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="17" operator="equal">
-      <formula>0.95</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="18" operator="between">
-      <formula>0.5</formula>
-      <formula>0.9</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="19" operator="between">
-      <formula>0.9</formula>
-      <formula>0.9499999</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="greaterThan">
-      <formula>0.95</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K6:K12">
-    <cfRule type="cellIs" dxfId="14" priority="11" operator="lessThan">
-      <formula>0.5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="12" operator="equal">
-      <formula>0.95</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="between">
-      <formula>0.5</formula>
-      <formula>0.9</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="14" operator="between">
-      <formula>0.9</formula>
-      <formula>0.9499999</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="15" operator="greaterThan">
-      <formula>0.95</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K16:K22">
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="lessThan">
-      <formula>0.5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
-      <formula>0.95</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="between">
-      <formula>0.5</formula>
-      <formula>0.9</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="between">
-      <formula>0.9</formula>
-      <formula>0.9499999</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="10" operator="greaterThan">
-      <formula>0.95</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V16:V22">
+  <conditionalFormatting sqref="K26:K32">
     <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>

</xml_diff>